<commit_message>
Testing Apache POI framework
</commit_message>
<xml_diff>
--- a/src/test/resources/DataFiles/Ebay_project_ExcelSheets.xlsx
+++ b/src/test/resources/DataFiles/Ebay_project_ExcelSheets.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="39">
   <si>
     <t>email</t>
   </si>
@@ -205,12 +205,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
@@ -612,7 +613,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>